<commit_message>
Updated with Motor configurator
</commit_message>
<xml_diff>
--- a/Details/ALADIN Details.xlsx
+++ b/Details/ALADIN Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://danfoss-my.sharepoint.com/personal/asish_george_danfoss_com/Documents/Shared Folders/Danfoss/ALADIN/Details/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC1048C821184BB45ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{085020B0-799E-4D93-B23F-15624BF61DAE}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_F25DC773A252ABDACC1048C821184BB45ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E362A0C4-AA58-4F13-86DE-1FFD9EC9274B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Options</t>
   </si>
   <si>
-    <t>open loop, closed loop</t>
-  </si>
-  <si>
     <t>Param 100</t>
   </si>
   <si>
@@ -93,18 +90,12 @@
     <t>Drop Down Input</t>
   </si>
   <si>
-    <t>U/F, VVC+</t>
-  </si>
-  <si>
     <t>Param 101</t>
   </si>
   <si>
     <t>Motor construction</t>
   </si>
   <si>
-    <t xml:space="preserve"> [0] asynchron [1] PM, non salient SPM [2] PM, salient IPM [5] SynRM [6] PMaSynRM</t>
-  </si>
-  <si>
     <t>Param 110</t>
   </si>
   <si>
@@ -133,13 +124,22 @@
   </si>
   <si>
     <t>Param 417</t>
+  </si>
+  <si>
+    <t>Open loop [0], Closed loop [3]</t>
+  </si>
+  <si>
+    <t>U/F [0], VVC+ [1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Asynchron [0] , PM - non salient SPM [1], PM - salient IPM [2] , SynRM [5],  PMaSynRM [6]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,13 +155,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -188,6 +200,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +485,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,95 +598,96 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
         <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;10&amp;K000000 Classified as Business</oddFooter>
   </headerFooter>

</xml_diff>